<commit_message>
Add code defects and solved in code
</commit_message>
<xml_diff>
--- a/Docs/lab1/CheckLists/Lab01_ReviewReport.xlsx
+++ b/Docs/lab1/CheckLists/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laptop\e\VVSS\CamiVVSS_ro2024-2025\Labs\Lab01\CheckListsAll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristiticu/Projects/vvss-public/Docs/lab1/CheckLists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C988F33-E974-4516-BC95-27D0B68ECC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5654333-3ABB-CA43-AE9D-6C43DDFC7373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -71,9 +71,6 @@
     <t xml:space="preserve">Author Name: </t>
   </si>
   <si>
-    <t>Popescu Ionel</t>
-  </si>
-  <si>
     <t>Georgescu Anca</t>
   </si>
   <si>
@@ -135,6 +132,63 @@
   </si>
   <si>
     <t>Effort to perform tool-based code analysis (hours):</t>
+  </si>
+  <si>
+    <t>Cristian Ticu</t>
+  </si>
+  <si>
+    <t>C05</t>
+  </si>
+  <si>
+    <t>OrdersGUIController, 107</t>
+  </si>
+  <si>
+    <t>Static method is called for an instance</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>Generic type called without parameters</t>
+  </si>
+  <si>
+    <t>OrdersGUIController, 25, 27, 29, 31</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t>OrdersGUIController, 55</t>
+  </si>
+  <si>
+    <t>Static field is accesed and modified for an instance</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>KitchenGUIController, 53</t>
+  </si>
+  <si>
+    <t>"startedAt" string is always concatenated instead of replacing old text</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>Variable names are cryptic and hard to understand</t>
+  </si>
+  <si>
+    <t>PizzaService, 31-36</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>KitchenGUIController, 21</t>
+  </si>
+  <si>
+    <t>"now" variable is evaluated only once and reused</t>
   </si>
 </sst>
 </file>
@@ -326,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -356,6 +410,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -398,7 +453,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,95 +770,95 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.90625" style="6"/>
+    <col min="1" max="1" width="8.83203125" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.5" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.83203125" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.90625" style="6"/>
+    <col min="10" max="10" width="14.5" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="H1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H3" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="24"/>
+      <c r="D4" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="25"/>
       <c r="H4" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="26"/>
+      <c r="D5" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="27"/>
       <c r="H5" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -814,7 +872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -822,7 +880,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -831,7 +889,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -840,7 +898,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -849,7 +907,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -858,7 +916,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -867,7 +925,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -876,7 +934,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -885,7 +943,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -894,7 +952,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -903,7 +961,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -912,7 +970,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -921,7 +979,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -930,7 +988,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -939,7 +997,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -948,7 +1006,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -957,7 +1015,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
@@ -985,98 +1043,98 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.90625" style="6"/>
-    <col min="9" max="9" width="22.08984375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="6"/>
+    <col min="1" max="1" width="8.83203125" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.5" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.83203125" style="6"/>
+    <col min="9" max="9" width="22.1640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="H1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H3" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="27"/>
+      <c r="D4" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="28"/>
       <c r="H4" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="29"/>
+      <c r="D5" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1090,7 +1148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1098,7 +1156,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1107,7 +1165,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1116,7 +1174,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1125,7 +1183,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1134,7 +1192,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1143,7 +1201,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1152,7 +1210,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1161,7 +1219,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1170,7 +1228,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1179,7 +1237,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1188,7 +1246,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1197,7 +1255,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1206,7 +1264,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1215,7 +1273,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1224,7 +1282,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1233,7 +1291,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1242,7 +1300,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
@@ -1270,99 +1328,107 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.90625" style="6"/>
-    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="6"/>
+    <col min="5" max="5" width="41.5" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.83203125" style="6"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="H1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="I3" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="17">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="30"/>
+      <c r="D4" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="32"/>
+      <c r="D5" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="33"/>
       <c r="H5" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="22"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D7" s="37">
+        <v>45728</v>
+      </c>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1376,69 +1442,102 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C12" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1447,16 +1546,13 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1465,25 +1561,19 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1492,7 +1582,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1501,7 +1591,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1510,7 +1600,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1519,7 +1609,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1528,7 +1618,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1537,7 +1627,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1546,7 +1636,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1555,7 +1645,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1564,7 +1654,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
@@ -1592,107 +1682,107 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.90625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.90625" style="6"/>
-    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="6"/>
+    <col min="5" max="5" width="23.83203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.83203125" style="6"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="H1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H3" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C4" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+        <v>24</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
       <c r="H5" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1701,7 +1791,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1711,7 +1801,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1721,7 +1811,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1731,7 +1821,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1741,7 +1831,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1751,7 +1841,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1761,7 +1851,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1771,7 +1861,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1781,7 +1871,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1791,7 +1881,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1801,7 +1891,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1811,7 +1901,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1821,7 +1911,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1831,7 +1921,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1841,7 +1931,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1851,7 +1941,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1861,7 +1951,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1871,7 +1961,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1881,7 +1971,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1891,7 +1981,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1901,16 +1991,16 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C32" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C32" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
       <c r="F32" s="18"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F35" s="35"/>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F35" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
checklist requirements, 1/2 checklist architectural, requirements_v2, PaymentRepository modified, completat raport aferent acestora
</commit_message>
<xml_diff>
--- a/Docs/lab1/CheckLists/Lab01_ReviewReport.xlsx
+++ b/Docs/lab1/CheckLists/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laptop\e\VVSS\CamiVVSS_ro2024-2025\Labs\Lab01\CheckListsAll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\programare\VVSS\lab1\gitul\vvss-public\Docs\lab1\CheckLists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C988F33-E974-4516-BC95-27D0B68ECC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A7115C-F2E2-4D2A-9CC8-E9088F9376ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="650" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -134,20 +134,153 @@
     <t>Tool-based Code Analysis</t>
   </si>
   <si>
-    <t>Effort to perform tool-based code analysis (hours):</t>
+    <t>Vasilief Andrei</t>
+  </si>
+  <si>
+    <t>12.03.2025</t>
+  </si>
+  <si>
+    <t>Ticu Cristian</t>
+  </si>
+  <si>
+    <t>R05</t>
+  </si>
+  <si>
+    <t>Care inchidere a restaurantului ? Se va afisa totalul incasarilor realizate vreodata, norml ar trebui pentru ziua/sesiunea respectiva</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>Ce se intampla daca un client face comanda, apoi mai vrea sa comande ceva ? Nu este mentionata aceasta obtiune, se vorbeste doar despre plasarea unei comenzi noi</t>
+  </si>
+  <si>
+    <t>R07</t>
+  </si>
+  <si>
+    <t>Nu se mentioneaza ce fel de arhitectura are aplicatia (daca este stratificata sau nu) si nu se mentioneaza nici in ce ordine face bucatarul pizzele, daca are un queue sau alta structura de date</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>Lipseste mecanismul de inchidere a bucatariei cu verificarile aferente</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>Nu exista, de exemplu ce se intampla daca esueaza plata cu cardul ?</t>
+  </si>
+  <si>
+    <t>SonarQube</t>
+  </si>
+  <si>
+    <t>12.03.2024</t>
+  </si>
+  <si>
+    <t>Use try-with-resources or close this "BufferedReader" in a "finally" clause.</t>
+  </si>
+  <si>
+    <t>Use try-with-resources or close this "BufferedWriter" in a "finally" clause.</t>
+  </si>
+  <si>
+    <t>This block of commented-out lines of code should be removed.</t>
+  </si>
+  <si>
+    <t>Replace this use of System.out by a logger.</t>
+  </si>
+  <si>
+    <t>Combine this catch with the one at line 32, which has the same body</t>
+  </si>
+  <si>
+    <t>PaymentRepository, 25</t>
+  </si>
+  <si>
+    <t>PaymentRepository, 65</t>
+  </si>
+  <si>
+    <t>PaymentRepository, 21</t>
+  </si>
+  <si>
+    <t>PaymentRepository, 67</t>
+  </si>
+  <si>
+    <t>PaymentRepository, 34</t>
+  </si>
+  <si>
+    <t>catch (FileNotFoundException e) {
+            e.printStackTrace();
+        } catch (IOException e) {
+            e.printStackTrace();
+        }</t>
+  </si>
+  <si>
+    <t>catch ( IOException e) {
+            e.printStackTrace();
+        }</t>
+  </si>
+  <si>
+    <t>Probabil exista un motiv pentru care afisam pe ecran si nu avem logger inca</t>
+  </si>
+  <si>
+    <t>Poate avem nevoie de acea liie de cod si trebuie sa o decomentam la un moment dat</t>
+  </si>
+  <si>
+    <t>try (BufferedReader br = new BufferedReader(new FileReader(file))) {
+    String line;
+    while ((line = br.readLine()) != null) {
+        Payment payment = getPayment(line);
+        paymentList.add(payment);
+    }
+} catch (IOException e) {
+    e.printStackTrace();
+}</t>
+  </si>
+  <si>
+    <t>BufferedReader br = null;
+        try {
+            br = new BufferedReader(new FileReader(file));
+            String line = null;
+            while((line=br.readLine())!=null){
+                Payment payment=getPayment(line);
+                paymentList.add(payment);
+            }
+            br.close();
+        } catch ( IOException e) {
+            e.printStackTrace();
+        }</t>
+  </si>
+  <si>
+    <t>BufferedWriter bw = null;
+        try {
+            bw = new BufferedWriter(new FileWriter(file));</t>
+  </si>
+  <si>
+    <t>try(BufferedWriter bw = new BufferedWriter(new FileWriter(file)))</t>
+  </si>
+  <si>
+    <t>Effort to perform tool-based code analysis (hours): 0.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -326,79 +459,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,8 +842,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -729,19 +863,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -754,31 +888,39 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="I3" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="17">
+        <v>237</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="25"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="3">
+        <v>237</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="27"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -790,15 +932,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
@@ -814,31 +960,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1">
+        <v>14</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
@@ -985,8 +1149,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1005,19 +1169,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1030,31 +1194,39 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="I3" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="17">
+        <v>237</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="3">
+        <v>237</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1066,15 +1238,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
@@ -1090,22 +1266,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E10" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
@@ -1291,19 +1475,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1323,10 +1507,10 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1337,10 +1521,10 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1352,15 +1536,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
@@ -1592,8 +1776,8 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1614,19 +1798,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1639,27 +1823,39 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="I3" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="17">
+        <v>237</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="D4" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="3">
+        <v>237</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="D5" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="22"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1671,8 +1867,10 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="22"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1692,54 +1890,90 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="333.5" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F12" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F13" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
@@ -1902,15 +2136,15 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C32" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
+      <c r="C32" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
       <c r="F32" s="18"/>
     </row>
     <row r="35" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F35" s="35"/>
+      <c r="F35" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Add architectural defects, sonarqube review and sonarqube implementations
</commit_message>
<xml_diff>
--- a/Docs/lab1/CheckLists/Lab01_ReviewReport.xlsx
+++ b/Docs/lab1/CheckLists/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristiticu/Projects/vvss-public/Docs/lab1/CheckLists/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\Desktop\Main Storage\coding_archive\uni\y3s2\vvss-public\Docs\lab1\CheckLists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5654333-3ABB-CA43-AE9D-6C43DDFC7373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A4D44F-E822-4077-A873-9E6EDABCEF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13023" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -189,19 +189,83 @@
   </si>
   <si>
     <t>"now" variable is evaluated only once and reused</t>
+  </si>
+  <si>
+    <t>Ticu Cristian</t>
+  </si>
+  <si>
+    <t>SonarQube for IDE</t>
+  </si>
+  <si>
+    <t>OrdersGUIController, 54</t>
+  </si>
+  <si>
+    <t>Instance methods should not write to "static" fields (java:S2696)</t>
+  </si>
+  <si>
+    <t>public void setTotalAmount(double totalAmount)</t>
+  </si>
+  <si>
+    <t>public static void setTotalAmount(double totalAmount)</t>
+  </si>
+  <si>
+    <t>OrdersGUIController, 59</t>
+  </si>
+  <si>
+    <t>Private fields only used as local variables in methods should become local variables (java:S1450)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    private int tableNumber;</t>
+  </si>
+  <si>
+    <t>SonarQube is wrong, variable is specific to instance</t>
+  </si>
+  <si>
+    <t>OrdersGUIController, 63</t>
+  </si>
+  <si>
+    <t>private ObservableList&lt;MenuDataModel&gt; menuData;</t>
+  </si>
+  <si>
+    <t>OrdersGUIController, 62</t>
+  </si>
+  <si>
+    <t>The diamond operator ("&lt;&gt;") should be used (java:S2293)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    private TableView&lt;MenuDataModel&gt; table = new TableView&lt;MenuDataModel&gt;();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    private TableView&lt;MenuDataModel&gt; table = new TableView&lt;&gt;();</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>No class descriptions (comments) are provided</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -380,82 +444,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,36 +835,36 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="6"/>
+    <col min="1" max="1" width="8.77734375" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.5" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.83203125" style="6"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.77734375" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.5" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="6"/>
+    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.77734375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15.65" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -808,57 +873,57 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="27"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="29"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -872,7 +937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -880,7 +945,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -889,7 +954,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -898,7 +963,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -907,7 +972,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -916,7 +981,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -925,7 +990,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -934,7 +999,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -943,7 +1008,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -952,7 +1017,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -961,7 +1026,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -970,7 +1035,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -979,7 +1044,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -988,7 +1053,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -997,7 +1062,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1006,7 +1071,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1015,7 +1080,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
@@ -1043,39 +1108,39 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="6"/>
+    <col min="1" max="1" width="8.77734375" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.5" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.83203125" style="6"/>
-    <col min="9" max="9" width="22.1640625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="6"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.77734375" style="6"/>
+    <col min="9" max="9" width="22.109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15.65" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -1084,57 +1149,57 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="30"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="32"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1148,7 +1213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1156,7 +1221,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1165,7 +1230,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1174,7 +1239,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1183,7 +1248,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1192,7 +1257,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1201,7 +1266,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1210,16 +1275,22 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1228,7 +1299,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1237,7 +1308,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1246,7 +1317,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1255,7 +1326,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1264,7 +1335,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1273,7 +1344,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1282,7 +1353,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1291,7 +1362,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1300,7 +1371,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
@@ -1328,40 +1399,40 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+    <sheetView zoomScale="136" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="6"/>
+    <col min="1" max="1" width="8.77734375" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.5" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.83203125" style="6"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.77734375" style="6"/>
     <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="6"/>
+    <col min="10" max="16384" width="8.77734375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15.65" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -1370,65 +1441,65 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="22" t="s">
         <v>32</v>
       </c>
       <c r="J3" s="17">
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="36"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="33">
         <v>45728</v>
       </c>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E7" s="24"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1442,7 +1513,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="30.05" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1456,7 +1527,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="30.05" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1471,7 +1542,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1486,7 +1557,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="30.05" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1501,7 +1572,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="30.05" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1516,7 +1587,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1531,13 +1602,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1546,13 +1617,13 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1561,19 +1632,19 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1582,7 +1653,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1591,7 +1662,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1600,7 +1671,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1609,7 +1680,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1618,7 +1689,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1627,7 +1698,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1636,7 +1707,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1645,7 +1716,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1654,7 +1725,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
@@ -1683,40 +1754,40 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="6"/>
+    <col min="1" max="1" width="8.77734375" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" style="6" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.83203125" style="6"/>
+    <col min="7" max="8" width="8.77734375" style="6"/>
     <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="6"/>
+    <col min="10" max="16384" width="8.77734375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15.65" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -1725,47 +1796,53 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I3" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="17">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="D4" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1782,46 +1859,78 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="60.1" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="45.1" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="75.150000000000006" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1831,7 +1940,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1841,7 +1950,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1851,7 +1960,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1861,7 +1970,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1871,7 +1980,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1881,7 +1990,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1891,7 +2000,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1901,7 +2010,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1911,7 +2020,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1921,7 +2030,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1931,7 +2040,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1941,7 +2050,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1951,7 +2060,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1961,7 +2070,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1971,7 +2080,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1981,7 +2090,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1991,15 +2100,15 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C32" s="34" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="18"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F35" s="21"/>
     </row>
   </sheetData>

</xml_diff>